<commit_message>
Version 3 Summary working
</commit_message>
<xml_diff>
--- a/Version 3/Cards/Audit-Input-keywordFile.xlsx
+++ b/Version 3/Cards/Audit-Input-keywordFile.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{7E78A68B-077B-4841-AA7D-9A941810C004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AAB9B072-E9FE-4D73-8895-64912A81C7B8}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{7E78A68B-077B-4841-AA7D-9A941810C004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6F7FCA70-02FA-49E3-8338-776A5336C238}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="3630" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InputFile" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="189">
   <si>
     <t>Mellanox InfiniBand and Ethernet Driver</t>
   </si>
@@ -316,9 +316,6 @@
   </si>
   <si>
     <t>HPE Apollo 9000 InfiniBand HDR 940z FIO Mezzanine Adapter (Comal)</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t xml:space="preserve">872726-B21 </t>
@@ -1108,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE18B724-FDB9-4FB6-BA51-2CC384B735F8}">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1155,7 +1152,7 @@
         <v>77</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>64</v>
@@ -1478,18 +1475,18 @@
         <v>87</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>85</v>
@@ -1527,13 +1524,13 @@
     </row>
     <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="C10" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>85</v>
@@ -1542,7 +1539,7 @@
         <v>86</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>87</v>
@@ -1566,18 +1563,18 @@
         <v>87</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>85</v>
@@ -1610,18 +1607,18 @@
         <v>87</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>110</v>
-      </c>
       <c r="C12" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>85</v>
@@ -1659,13 +1656,13 @@
     </row>
     <row r="13" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>85</v>
@@ -1703,13 +1700,13 @@
     </row>
     <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="C14" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>85</v>
@@ -1747,13 +1744,13 @@
     </row>
     <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>118</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>85</v>
@@ -1791,13 +1788,13 @@
     </row>
     <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>120</v>
-      </c>
       <c r="C16" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>85</v>
@@ -1835,13 +1832,13 @@
     </row>
     <row r="17" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>122</v>
-      </c>
       <c r="C17" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>85</v>
@@ -1879,13 +1876,13 @@
     </row>
     <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>124</v>
-      </c>
       <c r="C18" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>85</v>
@@ -1923,13 +1920,13 @@
     </row>
     <row r="19" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>126</v>
-      </c>
       <c r="C19" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>85</v>
@@ -1967,13 +1964,13 @@
     </row>
     <row r="20" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="C20" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>85</v>
@@ -2006,21 +2003,21 @@
         <v>87</v>
       </c>
       <c r="N20" s="11" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C21" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>86</v>
@@ -2055,16 +2052,16 @@
     </row>
     <row r="22" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>133</v>
-      </c>
       <c r="C22" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>86</v>
@@ -2099,16 +2096,16 @@
     </row>
     <row r="23" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>135</v>
-      </c>
       <c r="C23" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>86</v>
@@ -2143,16 +2140,16 @@
     </row>
     <row r="24" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>137</v>
-      </c>
       <c r="C24" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>86</v>
@@ -2182,21 +2179,21 @@
         <v>87</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>140</v>
-      </c>
       <c r="D25" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>86</v>
@@ -2231,16 +2228,16 @@
     </row>
     <row r="26" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>142</v>
-      </c>
       <c r="C26" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>86</v>
@@ -2275,16 +2272,16 @@
     </row>
     <row r="27" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>144</v>
-      </c>
       <c r="C27" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>86</v>
@@ -2319,16 +2316,16 @@
     </row>
     <row r="28" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C28" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="D28" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>86</v>
@@ -2363,16 +2360,16 @@
     </row>
     <row r="29" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>150</v>
-      </c>
       <c r="C29" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>86</v>
@@ -2407,16 +2404,16 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>153</v>
-      </c>
       <c r="D30" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>86</v>
@@ -2451,16 +2448,16 @@
     </row>
     <row r="31" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>155</v>
-      </c>
       <c r="C31" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>86</v>
@@ -2495,16 +2492,16 @@
     </row>
     <row r="32" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>157</v>
-      </c>
       <c r="C32" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>86</v>
@@ -2539,16 +2536,16 @@
     </row>
     <row r="33" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>159</v>
-      </c>
       <c r="C33" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>86</v>
@@ -2583,16 +2580,16 @@
     </row>
     <row r="34" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>161</v>
-      </c>
       <c r="C34" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>86</v>
@@ -2627,16 +2624,16 @@
     </row>
     <row r="35" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>163</v>
-      </c>
       <c r="C35" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>86</v>
@@ -2671,16 +2668,16 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>165</v>
-      </c>
       <c r="C36" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>86</v>
@@ -2715,16 +2712,16 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>167</v>
-      </c>
       <c r="C37" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>86</v>
@@ -2759,16 +2756,16 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>169</v>
-      </c>
       <c r="C38" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>86</v>
@@ -2803,16 +2800,16 @@
     </row>
     <row r="39" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="C39" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>86</v>
@@ -2847,16 +2844,16 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>173</v>
-      </c>
       <c r="C40" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>86</v>
@@ -2891,16 +2888,16 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>175</v>
-      </c>
       <c r="C41" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>86</v>
@@ -2935,10 +2932,10 @@
     </row>
     <row r="42" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>177</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>84</v>
@@ -2979,10 +2976,10 @@
     </row>
     <row r="43" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>84</v>
@@ -3023,10 +3020,10 @@
     </row>
     <row r="44" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>181</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>84</v>
@@ -3067,10 +3064,10 @@
     </row>
     <row r="45" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>182</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>183</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>84</v>
@@ -3111,16 +3108,16 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="C46" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>186</v>
-      </c>
       <c r="D46" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>86</v>
@@ -3155,16 +3152,16 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>188</v>
-      </c>
       <c r="C47" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>86</v>

</xml_diff>